<commit_message>
updated team report to reflect completion
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="168">
   <si>
     <t>Initials</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Coding-need output format &amp; test case</t>
   </si>
   <si>
     <t>Keep doing:</t>
@@ -666,7 +669,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -741,7 +744,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -776,9 +779,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -791,7 +792,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -802,7 +803,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -811,9 +812,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -826,7 +825,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -835,16 +834,68 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -916,11 +967,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="11729647"/>
-        <c:axId val="18264443"/>
+        <c:axId val="99510627"/>
+        <c:axId val="7823894"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11729647"/>
+        <c:axId val="99510627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,14 +1007,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18264443"/>
+        <c:crossAx val="7823894"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18264443"/>
+        <c:axId val="7823894"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +1060,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11729647"/>
+        <c:crossAx val="99510627"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1041,15 +1092,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>145080</xdr:colOff>
+      <xdr:colOff>172080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>451080</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:colOff>477720</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1057,8 +1108,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="983160" y="1463400"/>
-        <a:ext cx="4668480" cy="2670840"/>
+        <a:off x="991080" y="1454400"/>
+        <a:ext cx="4591800" cy="2670480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1078,16 +1129,16 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="6.14285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.0803571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="6.02232142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.84375"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,17 +1236,17 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.84375"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72321428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,13 +1572,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1651785714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.61607142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1651785714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.49553571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,22 +1653,22 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.09375"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.09375"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.61607142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,7 +1759,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>10</v>
@@ -1733,6 +1784,15 @@
       <c r="F6" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1750,11 +1810,20 @@
       <c r="F7" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,7 +1846,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1860,7 @@
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1819,7 +1888,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1875,7 +1944,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,7 +2000,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,15 +2051,15 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.15625"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="48.1919642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.92410714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="47.71875"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2001,7 +2070,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,7 +2081,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,7 +2092,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2103,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2114,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,7 +2125,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,7 +2136,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2078,7 +2147,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,7 +2158,7 @@
         <v>42</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,7 +2169,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,7 +2180,7 @@
         <v>46</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,7 +2191,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,7 +2202,7 @@
         <v>50</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2213,7 @@
         <v>52</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,7 +2224,7 @@
         <v>54</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,7 +2235,7 @@
         <v>56</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,7 +2246,7 @@
         <v>58</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,7 +2257,7 @@
         <v>60</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,7 +2268,7 @@
         <v>62</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2210,7 +2279,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,7 +2290,7 @@
         <v>66</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,7 +2301,7 @@
         <v>68</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2312,7 @@
         <v>70</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,7 +2323,7 @@
         <v>72</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,205 +2334,205 @@
         <v>74</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated team report to reflect US03
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="570" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,16 +18,11 @@
     <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
   <si>
     <t>Initials</t>
   </si>
@@ -285,6 +280,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Coding-verify output format with team</t>
   </si>
   <si>
     <t>Coding-need output format &amp; test case</t>
@@ -669,7 +667,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -744,12 +742,12 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
@@ -767,142 +765,14 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
-              </a:solidFill>
-            </c:spPr>
+            <c:size val="4"/>
           </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -957,27 +827,18 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="99510627"/>
-        <c:axId val="7823894"/>
+        <c:axId val="49412610"/>
+        <c:axId val="91238347"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99510627"/>
+        <c:axId val="49412610"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="M/D" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -989,32 +850,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="7823894"/>
+        <c:crossAx val="91238347"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7823894"/>
+        <c:axId val="91238347"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,7 +873,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1042,27 +884,8 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="99510627"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossAx val="49412610"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1074,7 +897,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1092,15 +914,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>172080</xdr:colOff>
+      <xdr:colOff>199080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>125280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>477720</xdr:colOff>
+      <xdr:colOff>504720</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1108,8 +930,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="991080" y="1454400"/>
-        <a:ext cx="4591800" cy="2670480"/>
+        <a:off x="1018080" y="1445760"/>
+        <a:ext cx="4911840" cy="2670120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1567,14 +1389,14 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.15625"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0089285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9553571428571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.73214285714286"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.49553571428571"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9285714285714"/>
@@ -1654,7 +1476,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -1667,7 +1489,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.97767857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.38839285714286"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.7991071428571"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
@@ -1750,6 +1572,15 @@
       <c r="F4" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1759,7 +1590,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>10</v>
@@ -1791,7 +1622,7 @@
         <v>40</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,7 +1648,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1677,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +1691,7 @@
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2051,10 +1882,10 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.92410714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8616071428571"/>
@@ -2062,7 +1893,7 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.92410714285714"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2070,10 +1901,10 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
@@ -2081,10 +1912,10 @@
         <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>29</v>
       </c>
@@ -2092,10 +1923,10 @@
         <v>30</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
@@ -2103,10 +1934,10 @@
         <v>32</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
@@ -2114,10 +1945,10 @@
         <v>34</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
@@ -2125,10 +1956,10 @@
         <v>36</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
@@ -2136,10 +1967,10 @@
         <v>38</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>39</v>
       </c>
@@ -2147,10 +1978,10 @@
         <v>40</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>41</v>
       </c>
@@ -2158,10 +1989,10 @@
         <v>42</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>43</v>
       </c>
@@ -2169,10 +2000,10 @@
         <v>44</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>45</v>
       </c>
@@ -2180,10 +2011,10 @@
         <v>46</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>47</v>
       </c>
@@ -2191,10 +2022,10 @@
         <v>48</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>49</v>
       </c>
@@ -2202,10 +2033,10 @@
         <v>50</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>51</v>
       </c>
@@ -2213,10 +2044,10 @@
         <v>52</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>53</v>
       </c>
@@ -2224,10 +2055,10 @@
         <v>54</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>55</v>
       </c>
@@ -2235,10 +2066,10 @@
         <v>56</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>57</v>
       </c>
@@ -2246,10 +2077,10 @@
         <v>58</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>59</v>
       </c>
@@ -2257,10 +2088,10 @@
         <v>60</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>61</v>
       </c>
@@ -2268,10 +2099,10 @@
         <v>62</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
@@ -2279,10 +2110,10 @@
         <v>64</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>65</v>
       </c>
@@ -2290,10 +2121,10 @@
         <v>66</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>67</v>
       </c>
@@ -2301,10 +2132,10 @@
         <v>68</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>69</v>
       </c>
@@ -2312,10 +2143,10 @@
         <v>70</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>71</v>
       </c>
@@ -2323,10 +2154,10 @@
         <v>72</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>73</v>
       </c>
@@ -2334,205 +2165,205 @@
         <v>74</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="44.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated report to reflect completion of US03 and US04
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="570" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="284" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="169">
   <si>
     <t>Initials</t>
   </si>
@@ -282,7 +282,7 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Coding-verify output format with team</t>
+    <t>Done</t>
   </si>
   <si>
     <t>Coding-need output format &amp; test case</t>
@@ -572,8 +572,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -667,7 +666,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="14" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -742,7 +741,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -765,7 +764,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -829,11 +828,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="49412610"/>
-        <c:axId val="91238347"/>
+        <c:axId val="79773814"/>
+        <c:axId val="92206655"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49412610"/>
+        <c:axId val="79773814"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,14 +849,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91238347"/>
+        <c:crossAx val="92206655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91238347"/>
+        <c:axId val="92206655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +883,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="49412610"/>
+        <c:crossAx val="79773814"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -914,15 +913,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>199080</xdr:colOff>
+      <xdr:colOff>226080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>504720</xdr:colOff>
+      <xdr:colOff>531360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -930,8 +929,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1018080" y="1445760"/>
-        <a:ext cx="4911840" cy="2670120"/>
+        <a:off x="1045080" y="1436760"/>
+        <a:ext cx="4911480" cy="2669760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1476,7 +1475,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -1597,6 +1596,15 @@
       </c>
       <c r="F5" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added owners and estimations for next Sprint post scrum
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr date1904="1" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\SSW-Agile-GEDCOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="468" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId1"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
-    <sheet name="Stories" sheetId="8" r:id="rId8"/>
+    <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Backlog" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Burndown" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sprint1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sprint2" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sprint3" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sprint4" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="172">
   <si>
     <t>Initials</t>
   </si>
@@ -286,16 +287,25 @@
     <t>Completed</t>
   </si>
   <si>
+    <t>Complete w/ tests</t>
+  </si>
+  <si>
     <t>Done</t>
   </si>
   <si>
-    <t>Coding-need output format &amp; test case</t>
-  </si>
-  <si>
     <t>Keep doing:</t>
   </si>
   <si>
+    <t>Code Reviews and consistency checks</t>
+  </si>
+  <si>
+    <t>PEP8</t>
+  </si>
+  <si>
     <t>Avoid:</t>
+  </si>
+  <si>
+    <t>assigned</t>
   </si>
   <si>
     <t>Story Description</t>
@@ -538,12 +548,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="M/D"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -551,11 +563,32 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -573,7 +606,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -581,37 +614,89 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="12">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="14"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -670,47 +755,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4a7ebb"/>
+            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
+                <a:srgbClr val="4a7ebb"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -718,42 +785,118 @@
           <c:marker>
             <c:symbol val="diamond"/>
             <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4a7ebb"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
-          <c:dLbls>
+          <c:dPt>
+            <c:idx val="0"/>
             <c:spPr>
-              <a:noFill/>
-              <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
             </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c">
+                  <a:alpha val="-1446784704"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="2067066720">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="2972724840">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff">
+                  <a:alpha val="-47148408"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="3109385880">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
+                  <c:v>9/22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>10/5</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -767,32 +910,42 @@
                 <c:pt idx="1">
                   <c:v>30</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-760897024"/>
-        <c:axId val="-760891040"/>
+        <c:axId val="79559722"/>
+        <c:axId val="36964873"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="-760897024"/>
+      <c:catAx>
+        <c:axId val="79559722"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="M/D" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -804,14 +957,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-760891040"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="36964873"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="-760891040"/>
+        <c:axId val="36964873"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +998,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -839,13 +1010,31 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-760897024"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="79559722"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -854,47 +1043,41 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>226080</xdr:colOff>
+      <xdr:colOff>253080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>107280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>531360</xdr:colOff>
+      <xdr:colOff>558000</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="0" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="1053000" y="1402560"/>
+        <a:ext cx="4838760" cy="2618640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -907,284 +1090,26 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="6"/>
-    <col min="3" max="3" width="8.25"/>
-    <col min="4" max="5" width="19.875"/>
-    <col min="6" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.90625"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1201,90 +1126,98 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.75"/>
-    <col min="2" max="2" width="7.25"/>
-    <col min="3" max="3" width="26.875"/>
-    <col min="4" max="4" width="6.375"/>
-    <col min="5" max="5" width="7.25"/>
-    <col min="6" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.60714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.25892857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1301,314 +1234,340 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="D10" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="D11" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="D12" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="D13" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.125"/>
-    <col min="2" max="2" width="18"/>
-    <col min="3" max="3" width="14"/>
-    <col min="4" max="4" width="6.75"/>
-    <col min="5" max="5" width="6.5"/>
-    <col min="6" max="6" width="11.875"/>
-    <col min="7" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.92410714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.71875"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.61607142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6919642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
@@ -1628,67 +1587,77 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
         <v>40442</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <v>40455</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="C3">
-        <f>B2-B3</f>
+      <c r="C3" s="0" t="n">
+        <f aca="false">B2-B3</f>
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="F3" s="5">
-        <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+      <c r="F3" s="5" t="n">
+        <f aca="false">(D3-D2)/E3*60</f>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.25"/>
-    <col min="2" max="2" width="23.875" style="6"/>
-    <col min="3" max="3" width="6.375"/>
-    <col min="4" max="4" width="6.625"/>
-    <col min="5" max="5" width="8.375"/>
-    <col min="7" max="7" width="8.375"/>
-    <col min="9" max="9" width="32.75"/>
-    <col min="10" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="23.5044642857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.25892857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.78125"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.3660714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1717,219 +1686,245 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="D2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="I2" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="D3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="I3" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="D4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="D7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F6">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>22</v>
-      </c>
-      <c r="H6">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="F7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>23</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.53125"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.6875"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7723214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1958,26 +1953,154 @@
         <v>85</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2007,25 +2130,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2055,28 +2186,36 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.875"/>
-    <col min="2" max="2" width="23.875"/>
-    <col min="3" max="3" width="47.75" style="6"/>
-    <col min="4" max="1025" width="9.875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5044642857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="141.834821428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2084,473 +2223,478 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C2" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C3" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C4" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C5" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C6" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="110.25" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C7" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C8" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C9" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C10" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C11" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C12" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C13" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C14" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C15" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C16" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C17" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C18" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C19" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C20" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="C21" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C22" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="C23" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C24" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="236.25" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="26" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B26" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="27" customFormat="false" ht="236.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B27" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C27" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="28" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B28" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="29" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B29" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C29" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="30" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B30" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C30" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="31" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B31" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C31" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="32" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B32" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C32" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="33" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B33" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C33" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="34" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B34" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="35" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B35" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C35" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="36" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B36" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C36" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="37" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B37" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C37" s="11" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="38" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B38" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C38" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="39" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B39" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C39" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="40" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B40" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C40" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="63" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="41" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B41" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C41" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="42" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B42" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C42" s="11" t="s">
         <v>168</v>
       </c>
     </row>
+    <row r="43" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated team report to reflect completion of Sprint 1
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="470" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,16 +18,11 @@
     <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -303,6 +298,9 @@
   </si>
   <si>
     <t>Avoid:</t>
+  </si>
+  <si>
+    <t>Code Duplication</t>
   </si>
   <si>
     <t>assigned</t>
@@ -763,9 +761,9 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
@@ -783,94 +781,14 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
-              </a:solidFill>
-            </c:spPr>
+            <c:size val="2"/>
           </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="6022292400">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="6035662080">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln w="2972724840">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -878,10 +796,10 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9/22</c:v>
+                  <c:v>2/15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10/5</c:v>
+                  <c:v>2/28</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -905,10 +823,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v/>
@@ -925,27 +843,18 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
         </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="79559722"/>
-        <c:axId val="36964873"/>
+        <c:axId val="85710002"/>
+        <c:axId val="76679543"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79559722"/>
+        <c:axId val="85710002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="M/D" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -957,32 +866,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="36964873"/>
+        <c:crossAx val="76679543"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36964873"/>
+        <c:axId val="76679543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,7 +889,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1010,27 +900,8 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="79559722"/>
+        <c:crossAx val="85710002"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1042,7 +913,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1060,15 +930,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>280080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>558000</xdr:colOff>
+      <xdr:colOff>584640</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>135000</xdr:rowOff>
+      <xdr:rowOff>125280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1076,8 +946,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1053000" y="1402560"/>
-        <a:ext cx="4838760" cy="2618640"/>
+        <a:off x="1080000" y="1393560"/>
+        <a:ext cx="4838400" cy="2618280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1203,7 +1073,7 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1553,7 +1423,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1589,35 +1459,47 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
-        <v>40442</v>
+        <v>40953</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
-        <v>40455</v>
+        <v>40966</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>30</v>
+        <f aca="false">42-6</f>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">B2-B3</f>
         <v>6</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>250</v>
+        <f aca="false">SUM(Sprint1!G2:G7)</f>
+        <v>142</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>120</v>
+        <f aca="false">MIN(Sprint1!G2:G7)</f>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="n">
         <f aca="false">(D3-D2)/E3*60</f>
-        <v>125</v>
+        <v>710</v>
       </c>
     </row>
   </sheetData>
@@ -1639,8 +1521,8 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1706,7 +1588,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>30</v>
@@ -1735,7 +1617,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>10</v>
@@ -1764,7 +1646,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>20</v>
@@ -1793,7 +1675,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>20</v>
@@ -1822,7 +1704,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>40</v>
@@ -1851,7 +1733,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>5</v>
@@ -1862,6 +1744,21 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7"/>
@@ -1892,7 +1789,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1964,7 +1865,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>30</v>
@@ -1984,7 +1885,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>30</v>
@@ -2004,7 +1905,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>30</v>
@@ -2024,7 +1925,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>30</v>
@@ -2044,7 +1945,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>45</v>
@@ -2064,7 +1965,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>30</v>
@@ -2203,7 +2104,7 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2223,7 +2124,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,7 +2135,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,7 +2146,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,7 +2157,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,7 +2168,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,7 +2179,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,7 +2190,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,7 +2201,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2212,7 @@
         <v>42</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2223,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,7 +2234,7 @@
         <v>46</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,7 +2245,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,7 +2256,7 @@
         <v>50</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,7 +2267,7 @@
         <v>52</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2377,7 +2278,7 @@
         <v>54</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,7 +2289,7 @@
         <v>56</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,7 +2300,7 @@
         <v>58</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2311,7 @@
         <v>60</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2322,7 @@
         <v>62</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,7 +2333,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,7 +2344,7 @@
         <v>66</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,7 +2355,7 @@
         <v>68</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,7 +2366,7 @@
         <v>70</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,7 +2377,7 @@
         <v>72</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2487,205 +2388,205 @@
         <v>74</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="236.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated team report to reflect US09
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="470" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="564" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -584,8 +584,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -758,7 +757,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -845,11 +844,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="85710002"/>
-        <c:axId val="76679543"/>
+        <c:axId val="2465932"/>
+        <c:axId val="70944275"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85710002"/>
+        <c:axId val="2465932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,14 +865,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="76679543"/>
+        <c:crossAx val="70944275"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76679543"/>
+        <c:axId val="70944275"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +899,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="85710002"/>
+        <c:crossAx val="2465932"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -930,15 +929,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>280080</xdr:colOff>
+      <xdr:colOff>307080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>97560</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>584640</xdr:colOff>
+      <xdr:colOff>611280</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -946,8 +945,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1080000" y="1393560"/>
-        <a:ext cx="4838400" cy="2618280"/>
+        <a:off x="1107000" y="1384560"/>
+        <a:ext cx="4838040" cy="2617920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1521,7 +1520,7 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1812,8 +1811,8 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1891,7 +1890,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,7 +1910,16 @@
         <v>30</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,7 +1939,7 @@
         <v>30</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1951,7 +1959,7 @@
         <v>45</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +1979,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating to reflect completed user stories. Also completed this sprints burndown
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -552,11 +552,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -589,6 +590,7 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -641,7 +643,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -666,11 +668,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,7 +696,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -801,9 +807,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -816,7 +820,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -827,7 +831,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -836,9 +840,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -851,7 +853,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -860,16 +862,68 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
+                <a:srgbClr val="83caff"/>
               </a:solidFill>
-              <a:ln w="3109385880">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -890,7 +944,7 @@
                   <c:v>2/28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>03/13/16</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -917,7 +971,7 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -941,11 +995,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="17303001"/>
-        <c:axId val="59783262"/>
+        <c:axId val="11034549"/>
+        <c:axId val="357926"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17303001"/>
+        <c:axId val="11034549"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,14 +1035,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59783262"/>
+        <c:crossAx val="357926"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59783262"/>
+        <c:axId val="357926"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1004,7 +1058,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1034,7 +1088,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17303001"/>
+        <c:crossAx val="11034549"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1066,15 +1120,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>334080</xdr:colOff>
+      <xdr:colOff>361080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>637920</xdr:colOff>
+      <xdr:colOff>664560</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>106560</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1082,8 +1136,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1114920" y="1375560"/>
-        <a:ext cx="4780800" cy="2617560"/>
+        <a:off x="1132560" y="1342080"/>
+        <a:ext cx="4722840" cy="2617200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1109,10 +1163,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.78571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.3705357142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.66964285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.1339285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1215,12 +1269,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.48660714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3392857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.14285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.37053571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.85267857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9866071428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.02232142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85267857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1556,21 +1610,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6875"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4821428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7008928571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.25892857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5758928571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2455357142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5848214285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.14285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,7 +1672,7 @@
         <v>40966</v>
       </c>
       <c r="B3" s="0" t="n">
-        <f aca="false">42-6</f>
+        <f aca="false">B2-6</f>
         <v>36</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -1636,6 +1690,31 @@
       <c r="F3" s="5" t="n">
         <f aca="false">(D3-D2)/E3*60</f>
         <v>710</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>40980</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">B3-6</f>
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">B3-B4</f>
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">SUM(Sprint2!G2:G7)</f>
+        <v>148</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">MIN(Sprint2!G2:G7)</f>
+        <v>42</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <f aca="false">(D4-D3)/E4*60</f>
+        <v>8.57142857142857</v>
       </c>
     </row>
   </sheetData>
@@ -1663,23 +1742,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="23.1517857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.14285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4732142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.0089285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.85267857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.7946428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.02232142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2366071428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.65625"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1688,19 +1767,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1897,13 +1976,13 @@
       <c r="B13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
+      <c r="B14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="7"/>
+      <c r="B15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1913,7 +1992,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1921,12 +2000,12 @@
       <c r="B19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1949,23 +2028,23 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.56696428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.56696428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5848214285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1974,19 +2053,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2097,6 +2176,15 @@
       </c>
       <c r="F6" s="0" t="n">
         <v>35</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,14 +2240,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2168,19 +2256,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2208,14 +2296,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2224,19 +2312,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2264,10 +2352,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.56696428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1517857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="140.325892857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7946428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="138.790178571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.45089285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,7 +2365,7 @@
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2288,7 +2376,7 @@
       <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2299,7 +2387,7 @@
       <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2310,7 +2398,7 @@
       <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2321,7 +2409,7 @@
       <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2332,7 +2420,7 @@
       <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2343,7 +2431,7 @@
       <c r="B7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2354,7 +2442,7 @@
       <c r="B8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2365,7 +2453,7 @@
       <c r="B9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2376,7 +2464,7 @@
       <c r="B10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2387,7 +2475,7 @@
       <c r="B11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2398,7 +2486,7 @@
       <c r="B12" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2409,7 +2497,7 @@
       <c r="B13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2420,7 +2508,7 @@
       <c r="B14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2431,7 +2519,7 @@
       <c r="B15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="13" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2442,7 +2530,7 @@
       <c r="B16" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2453,7 +2541,7 @@
       <c r="B17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2464,7 +2552,7 @@
       <c r="B18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2475,7 +2563,7 @@
       <c r="B19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="13" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2486,7 +2574,7 @@
       <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="13" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2497,7 +2585,7 @@
       <c r="B21" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2508,7 +2596,7 @@
       <c r="B22" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2519,7 +2607,7 @@
       <c r="B23" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="13" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2530,7 +2618,7 @@
       <c r="B24" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="13" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2541,7 +2629,7 @@
       <c r="B25" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="13" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2552,7 +2640,7 @@
       <c r="B26" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="13" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2563,7 +2651,7 @@
       <c r="B27" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2574,7 +2662,7 @@
       <c r="B28" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2585,7 +2673,7 @@
       <c r="B29" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2596,7 +2684,7 @@
       <c r="B30" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2607,7 +2695,7 @@
       <c r="B31" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="13" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2618,7 +2706,7 @@
       <c r="B32" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="13" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2629,7 +2717,7 @@
       <c r="B33" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2640,7 +2728,7 @@
       <c r="B34" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2651,7 +2739,7 @@
       <c r="B35" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2662,7 +2750,7 @@
       <c r="B36" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="13" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2673,7 +2761,7 @@
       <c r="B37" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2684,7 +2772,7 @@
       <c r="B38" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="13" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2695,7 +2783,7 @@
       <c r="B39" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="13" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2706,7 +2794,7 @@
       <c r="B40" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="13" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2717,7 +2805,7 @@
       <c r="B41" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="13" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2728,7 +2816,7 @@
       <c r="B42" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="13" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2739,7 +2827,7 @@
       <c r="B43" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="13" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated team report to reflect next sprint
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -995,11 +995,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="11034549"/>
-        <c:axId val="357926"/>
+        <c:axId val="94151066"/>
+        <c:axId val="29259696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11034549"/>
+        <c:axId val="94151066"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,14 +1035,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357926"/>
+        <c:crossAx val="29259696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357926"/>
+        <c:axId val="29259696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1088,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11034549"/>
+        <c:crossAx val="94151066"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1120,15 +1120,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>361080</xdr:colOff>
+      <xdr:colOff>388080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>664560</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1136,8 +1136,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1132560" y="1342080"/>
-        <a:ext cx="4722840" cy="2617200"/>
+        <a:off x="1149840" y="1333080"/>
+        <a:ext cx="4665600" cy="2616840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1163,10 +1163,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.66964285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.91517857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.1339285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.8973214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,17 +1264,17 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.37053571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9866071428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.02232142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.25446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6294642857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.90625"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,7 +1462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>3</v>
       </c>
@@ -1472,8 +1472,11 @@
       <c r="C14" s="0" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>3</v>
       </c>
@@ -1483,8 +1486,11 @@
       <c r="C15" s="0" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>3</v>
       </c>
@@ -1494,8 +1500,11 @@
       <c r="C16" s="0" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>3</v>
       </c>
@@ -1505,8 +1514,11 @@
       <c r="C17" s="0" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>3</v>
       </c>
@@ -1516,8 +1528,11 @@
       <c r="C18" s="0" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
@@ -1526,6 +1541,9 @@
       </c>
       <c r="C19" s="0" t="s">
         <v>62</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,18 +1631,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.56696428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2455357142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5848214285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.37946428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.14285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0089285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.25892857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.02232142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,16 +1760,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.7946428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.02232142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2366071428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.65625"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.4419642857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.90625"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.1830357142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,16 +2046,16 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.45089285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.45089285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3482142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,15 +2250,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1026785714286"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0401785714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,6 +2292,126 @@
       </c>
       <c r="I1" s="9" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2296,7 +2438,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,16 +2488,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.45089285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7946428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="138.790178571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4419642857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="137.254464285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed burndown chart in team report
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="971" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,11 +18,6 @@
     <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -643,7 +638,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -660,15 +655,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -775,9 +766,9 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
@@ -795,175 +786,38 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
             <c:size val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
-              </a:solidFill>
-            </c:spPr>
           </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="6407280">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="2067066720">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:f>Burndown!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2/15</c:v>
+                  <c:v>02/15/16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/28</c:v>
+                  <c:v>02/28/16</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>03/13/16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>Burndown!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>42</c:v>
                 </c:pt>
@@ -973,39 +827,21 @@
                 <c:pt idx="2">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
         </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="94151066"/>
-        <c:axId val="29259696"/>
+        <c:axId val="68539618"/>
+        <c:axId val="94474463"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94151066"/>
+        <c:axId val="68539618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="M/D" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1017,32 +853,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="29259696"/>
+        <c:crossAx val="94474463"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29259696"/>
+        <c:axId val="94474463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,7 +876,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1070,27 +887,8 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="94151066"/>
+        <c:crossAx val="68539618"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1102,7 +900,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1120,15 +917,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>388080</xdr:colOff>
+      <xdr:colOff>415080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>691200</xdr:colOff>
+      <xdr:colOff>717840</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1136,8 +933,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1149840" y="1333080"/>
-        <a:ext cx="4665600" cy="2616840"/>
+        <a:off x="1176840" y="1324080"/>
+        <a:ext cx="4665240" cy="2616480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1630,8 +1427,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1665,7 +1462,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>40953</v>
       </c>
@@ -1711,7 +1508,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="4" t="n">
         <v>40980</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -1761,7 +1558,7 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.4419642857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="22.4419642857143"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.90625"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.91517857142857"/>
@@ -1776,7 +1573,7 @@
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1785,19 +1582,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1994,13 +1791,13 @@
       <c r="B13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
+      <c r="B14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2010,7 +1807,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2018,12 +1815,12 @@
       <c r="B19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2045,7 +1842,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -2062,7 +1859,7 @@
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2071,19 +1868,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2269,7 +2066,7 @@
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2278,19 +2075,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2445,7 +2242,7 @@
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2454,19 +2251,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2496,7 +2293,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4419642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="137.254464285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="137.254464285714"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.33035714285714"/>
   </cols>
   <sheetData>
@@ -2507,7 +2304,7 @@
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2518,7 +2315,7 @@
       <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2529,7 +2326,7 @@
       <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2540,7 +2337,7 @@
       <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2551,7 +2348,7 @@
       <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2562,7 +2359,7 @@
       <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2573,7 +2370,7 @@
       <c r="B7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2584,7 +2381,7 @@
       <c r="B8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2595,7 +2392,7 @@
       <c r="B9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2606,7 +2403,7 @@
       <c r="B10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2617,7 +2414,7 @@
       <c r="B11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2628,7 +2425,7 @@
       <c r="B12" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2639,7 +2436,7 @@
       <c r="B13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2650,7 +2447,7 @@
       <c r="B14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2661,7 +2458,7 @@
       <c r="B15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2672,7 +2469,7 @@
       <c r="B16" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2683,7 +2480,7 @@
       <c r="B17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2694,7 +2491,7 @@
       <c r="B18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2705,7 +2502,7 @@
       <c r="B19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2716,7 +2513,7 @@
       <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2727,7 +2524,7 @@
       <c r="B21" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2738,7 +2535,7 @@
       <c r="B22" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2749,7 +2546,7 @@
       <c r="B23" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2760,7 +2557,7 @@
       <c r="B24" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2771,7 +2568,7 @@
       <c r="B25" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2782,7 +2579,7 @@
       <c r="B26" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2793,7 +2590,7 @@
       <c r="B27" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2804,7 +2601,7 @@
       <c r="B28" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2815,7 +2612,7 @@
       <c r="B29" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2826,7 +2623,7 @@
       <c r="B30" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2837,7 +2634,7 @@
       <c r="B31" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2848,7 +2645,7 @@
       <c r="B32" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2859,7 +2656,7 @@
       <c r="B33" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2870,7 +2667,7 @@
       <c r="B34" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2881,7 +2678,7 @@
       <c r="B35" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2892,7 +2689,7 @@
       <c r="B36" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2903,7 +2700,7 @@
       <c r="B37" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2914,7 +2711,7 @@
       <c r="B38" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="12" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2925,7 +2722,7 @@
       <c r="B39" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2936,7 +2733,7 @@
       <c r="B40" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2947,7 +2744,7 @@
       <c r="B41" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2958,7 +2755,7 @@
       <c r="B42" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2969,7 +2766,7 @@
       <c r="B43" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="12" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
committing US 7 and 8
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -1,28 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr date1904="1" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\SSW-Agile-GEDCOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="971" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="971" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Backlog" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Burndown" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sprint1" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sprint2" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Sprint3" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Sprint4" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Team" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
+    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
+    <sheet name="Stories" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -546,15 +550,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="M/D"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -562,32 +564,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -605,7 +586,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -613,93 +594,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -758,59 +687,93 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4a7ebb"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
+                <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="diamond"/>
             <c:size val="2"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Burndown!$A$2:$A$4</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>mm/dd/yy</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>02/15/16</c:v>
+                  <c:v>40953</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>02/28/16</c:v>
+                  <c:v>40966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>03/13/16</c:v>
+                  <c:v>40980</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -830,18 +793,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="68539618"/>
-        <c:axId val="94474463"/>
+        <c:smooth val="0"/>
+        <c:axId val="-568647424"/>
+        <c:axId val="-568640896"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="68539618"/>
+      <c:dateAx>
+        <c:axId val="-568647424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -853,14 +827,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="94474463"/>
+        <c:crossAx val="-568640896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="94474463"/>
+        <c:axId val="-568640896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,6 +850,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -887,12 +862,13 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68539618"/>
+        <c:crossAx val="-568647424"/>
         <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -900,20 +876,27 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -927,14 +910,14 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1176840" y="1324080"/>
-        <a:ext cx="4665240" cy="2616480"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -947,26 +930,284 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.55357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.67857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.8973214285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.33035714285714"/>
+    <col min="1" max="2" width="5.5"/>
+    <col min="3" max="3" width="7.625"/>
+    <col min="4" max="5" width="18.875"/>
+    <col min="6" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -983,98 +1224,90 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.25446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6294642857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.90625"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.33035714285714"/>
+    <col min="1" max="1" width="4.25"/>
+    <col min="2" max="2" width="6.75"/>
+    <col min="3" max="3" width="25.625"/>
+    <col min="4" max="4" width="5.875"/>
+    <col min="5" max="5" width="6.75"/>
+    <col min="6" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1091,358 +1324,350 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>3</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>4</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>4</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>4</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>4</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.45089285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0089285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.25892857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.02232142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3392857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.33035714285714"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="17"/>
+    <col min="3" max="3" width="13.5"/>
+    <col min="4" max="4" width="6.25"/>
+    <col min="5" max="5" width="6"/>
+    <col min="6" max="6" width="11.375"/>
+    <col min="7" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
@@ -1462,114 +1687,106 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>40953</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>42</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>40966</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">B2-6</f>
+      <c r="B3">
+        <f>B2-6</f>
         <v>36</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <f aca="false">B2-B3</f>
+      <c r="C3">
+        <f>B2-B3</f>
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">SUM(Sprint1!G2:G7)</f>
+      <c r="D3">
+        <f>SUM(Sprint1!G2:G7)</f>
         <v>142</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">MIN(Sprint1!G2:G7)</f>
+      <c r="E3">
+        <f>MIN(Sprint1!G2:G7)</f>
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <f aca="false">(D3-D2)/E3*60</f>
+      <c r="F3" s="5">
+        <f>(D3-D2)/E3*60</f>
         <v>710</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>40980</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <f aca="false">B3-6</f>
+      <c r="B4">
+        <f>B3-6</f>
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <f aca="false">B3-B4</f>
+      <c r="C4">
+        <f>B3-B4</f>
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">SUM(Sprint2!G2:G7)</f>
-        <v>148</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">MIN(Sprint2!G2:G7)</f>
-        <v>42</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">(D4-D3)/E4*60</f>
-        <v>8.57142857142857</v>
+      <c r="D4">
+        <f>SUM(Sprint2!G2:G7)</f>
+        <v>203</v>
+      </c>
+      <c r="E4">
+        <f>MIN(Sprint2!G2:G7)</f>
+        <v>22</v>
+      </c>
+      <c r="F4" s="5">
+        <f>(D4-D3)/E4*60</f>
+        <v>166.36363636363637</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="22.4419642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.90625"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.91517857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.91517857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.1830357142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.33035714285714"/>
+    <col min="1" max="1" width="6.75"/>
+    <col min="2" max="2" width="22.5" style="6"/>
+    <col min="3" max="3" width="5.875"/>
+    <col min="4" max="4" width="15"/>
+    <col min="5" max="5" width="7.875"/>
+    <col min="6" max="6" width="8.125"/>
+    <col min="7" max="7" width="7.875"/>
+    <col min="8" max="8" width="8.125"/>
+    <col min="9" max="9" width="31.125"/>
+    <col min="10" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1598,264 +1815,256 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>15</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>30</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>33</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>30</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>15</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3">
         <v>30</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>30</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>20</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>20</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5">
         <v>13</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>20</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>30</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>26</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>40</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>10</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>20</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>28</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>5</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5758928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.33035714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3482142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.33035714285714"/>
+    <col min="1" max="1" width="9.375"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="9.375"/>
+    <col min="9" max="9" width="13.375"/>
+    <col min="10" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1884,185 +2093,195 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="G3">
+        <v>33</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>30</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>25</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4">
         <v>62</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>35</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>30</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>35</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>44</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>50</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>25</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>42</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>30</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1026785714286"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.33035714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0401785714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.33035714285714"/>
+    <col min="1" max="1" width="9.375"/>
+    <col min="2" max="2" width="25.125"/>
+    <col min="3" max="8" width="9.375"/>
+    <col min="9" max="9" width="11"/>
+    <col min="10" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2091,154 +2310,146 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>45</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>45</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>45</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.33035714285714"/>
+    <col min="1" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2268,36 +2479,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4419642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="137.254464285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.33035714285714"/>
+    <col min="1" max="1" width="9.375"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="137.25" style="6"/>
+    <col min="4" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2308,462 +2511,462 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>64</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>66</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>120</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="236.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>123</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>126</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>128</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>129</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>131</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>132</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>134</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>135</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>138</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>140</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>141</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>144</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>146</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>147</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>150</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>153</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>155</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>156</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>159</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>161</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>162</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>164</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>165</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>168</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>170</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>171</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -2771,12 +2974,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed anomaly case for father dying within 9 months before child is born. This is not an anomaly. Also refactored some code.
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -1,32 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr date1904="1" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\SSW-Agile-GEDCOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="971" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="392" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId1"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
-    <sheet name="Stories" sheetId="8" r:id="rId8"/>
+    <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Backlog" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Burndown" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sprint1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sprint2" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sprint3" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sprint4" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="173">
   <si>
     <t>Initials</t>
   </si>
@@ -550,13 +546,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="M/D"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -564,11 +562,43 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -586,7 +616,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -594,41 +624,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -646,7 +728,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF878787"/>
+      <rgbColor rgb="FF8B8B8B"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -687,93 +769,79 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4a7ebb"/>
+            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
+                <a:srgbClr val="4a7ebb"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
             <c:size val="2"/>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Burndown!$A$2:$A$4</c:f>
-              <c:numCache>
-                <c:formatCode>mm/dd/yy</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>40953</c:v>
+                  <c:v>02/15/16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40966</c:v>
+                  <c:v>02/28/16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40980</c:v>
+                  <c:v>03/13/16</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -793,82 +861,99 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-568647424"/>
-        <c:axId val="-568640896"/>
+        <c:axId val="56388568"/>
+        <c:axId val="10066007"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="-568647424"/>
+      <c:catAx>
+        <c:axId val="56388568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln w="6480">
             <a:solidFill>
-              <a:srgbClr val="878787"/>
+              <a:srgbClr val="8b8b8b"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-568640896"/>
+        <c:crossAx val="10066007"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="-568640896"/>
+        <c:axId val="10066007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="878787"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Remaining Stories</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln w="6480">
             <a:solidFill>
-              <a:srgbClr val="878787"/>
+              <a:srgbClr val="8b8b8b"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-568647424"/>
+        <c:crossAx val="56388568"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -876,48 +961,41 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>415080</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:colOff>329400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>717840</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>499320</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="0" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="1095120" y="1180440"/>
+        <a:ext cx="5291280" cy="3263040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -930,284 +1008,26 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="5.5"/>
-    <col min="3" max="3" width="7.625"/>
-    <col min="4" max="5" width="18.875"/>
-    <col min="6" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.49553571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.62053571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.875"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1224,90 +1044,98 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.25"/>
-    <col min="2" max="2" width="6.75"/>
-    <col min="3" max="3" width="25.625"/>
-    <col min="4" max="4" width="5.875"/>
-    <col min="5" max="5" width="6.75"/>
-    <col min="6" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.25446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.625"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.875"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1324,350 +1152,358 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.5"/>
-    <col min="2" max="2" width="17"/>
-    <col min="3" max="3" width="13.5"/>
-    <col min="4" max="4" width="6.25"/>
-    <col min="5" max="5" width="6"/>
-    <col min="6" max="6" width="11.375"/>
-    <col min="7" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.49553571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4955357142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.25446428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3794642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>75</v>
       </c>
@@ -1687,106 +1523,114 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
         <v>40953</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <v>40966</v>
       </c>
-      <c r="B3">
-        <f>B2-6</f>
+      <c r="B3" s="0" t="n">
+        <f aca="false">B2-6</f>
         <v>36</v>
       </c>
-      <c r="C3">
-        <f>B2-B3</f>
+      <c r="C3" s="0" t="n">
+        <f aca="false">B2-B3</f>
         <v>6</v>
       </c>
-      <c r="D3">
-        <f>SUM(Sprint1!G2:G7)</f>
+      <c r="D3" s="0" t="n">
+        <f aca="false">SUM(Sprint1!G2:G7)</f>
         <v>142</v>
       </c>
-      <c r="E3">
-        <f>MIN(Sprint1!G2:G7)</f>
+      <c r="E3" s="0" t="n">
+        <f aca="false">MIN(Sprint1!G2:G7)</f>
         <v>12</v>
       </c>
-      <c r="F3" s="5">
-        <f>(D3-D2)/E3*60</f>
+      <c r="F3" s="5" t="n">
+        <f aca="false">(D3-D2)/E3*60</f>
         <v>710</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>40980</v>
       </c>
-      <c r="B4">
-        <f>B3-6</f>
+      <c r="B4" s="0" t="n">
+        <f aca="false">B3-6</f>
         <v>30</v>
       </c>
-      <c r="C4">
-        <f>B3-B4</f>
+      <c r="C4" s="0" t="n">
+        <f aca="false">B3-B4</f>
         <v>6</v>
       </c>
-      <c r="D4">
-        <f>SUM(Sprint2!G2:G7)</f>
-        <v>203</v>
-      </c>
-      <c r="E4">
-        <f>MIN(Sprint2!G2:G7)</f>
+      <c r="D4" s="0" t="n">
+        <f aca="false">SUM(Sprint2!G2:G7)</f>
+        <v>230</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">MIN(Sprint2!G2:G7)</f>
         <v>22</v>
       </c>
-      <c r="F4" s="5">
-        <f>(D4-D3)/E4*60</f>
-        <v>166.36363636363637</v>
+      <c r="F4" s="5" t="n">
+        <f aca="false">(D4-D3)/E4*60</f>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.75"/>
-    <col min="2" max="2" width="22.5" style="6"/>
-    <col min="3" max="3" width="5.875"/>
-    <col min="4" max="4" width="15"/>
-    <col min="5" max="5" width="7.875"/>
-    <col min="6" max="6" width="8.125"/>
-    <col min="7" max="7" width="7.875"/>
-    <col min="8" max="8" width="8.125"/>
-    <col min="9" max="9" width="31.125"/>
-    <col min="10" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="22.4955357142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.875"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.875"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.125"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.125"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.1294642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1815,256 +1659,264 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="9.375"/>
-    <col min="9" max="9" width="13.375"/>
-    <col min="10" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3794642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2093,195 +1945,239 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G4">
-        <v>62</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="G5" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="0" t="s">
         <v>85</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375"/>
-    <col min="2" max="2" width="25.125"/>
-    <col min="3" max="8" width="9.375"/>
-    <col min="9" max="9" width="11"/>
-    <col min="10" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1294642857143"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2310,146 +2206,154 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2479,28 +2383,36 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.375"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="137.25" style="6"/>
-    <col min="4" max="1025" width="9.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="137.254464285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.37946428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2511,462 +2423,462 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>66</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>120</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>123</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="0" t="s">
         <v>126</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="0" t="s">
         <v>129</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>132</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="0" t="s">
         <v>135</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="0" t="s">
         <v>138</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>141</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="0" t="s">
         <v>144</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="0" t="s">
         <v>147</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="0" t="s">
         <v>150</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="0" t="s">
         <v>153</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="0" t="s">
         <v>156</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="0" t="s">
         <v>159</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="0" t="s">
         <v>162</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="0" t="s">
         <v>165</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="0" t="s">
         <v>168</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="0" t="s">
         <v>171</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -2974,7 +2886,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
committing Team1Report.xlsx for finishing sprint 2
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="392" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="392" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -863,11 +863,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="56388568"/>
-        <c:axId val="10066007"/>
+        <c:axId val="30616361"/>
+        <c:axId val="76233007"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56388568"/>
+        <c:axId val="30616361"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,14 +904,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10066007"/>
+        <c:crossAx val="76233007"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10066007"/>
+        <c:axId val="76233007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -948,7 +948,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="56388568"/>
+        <c:crossAx val="30616361"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -978,15 +978,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>329400</xdr:colOff>
+      <xdr:colOff>356400</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>499320</xdr:colOff>
+      <xdr:colOff>525960</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -994,8 +994,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1095120" y="1180440"/>
-        <a:ext cx="5291280" cy="3263040"/>
+        <a:off x="1122120" y="1171440"/>
+        <a:ext cx="5290920" cy="3262680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1488,8 +1488,8 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1903,7 +1903,7 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more fixes to Team Report
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="392" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="785" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="175">
   <si>
     <t>Initials</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>assigned</t>
+  </si>
+  <si>
+    <t>Unnecessary features</t>
   </si>
   <si>
     <t>Story Description</t>
@@ -866,11 +869,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50006769"/>
-        <c:axId val="39931619"/>
+        <c:axId val="45722570"/>
+        <c:axId val="72546527"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50006769"/>
+        <c:axId val="45722570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,14 +910,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39931619"/>
+        <c:crossAx val="72546527"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39931619"/>
+        <c:axId val="72546527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +954,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50006769"/>
+        <c:crossAx val="45722570"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -981,15 +984,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>383400</xdr:colOff>
+      <xdr:colOff>410400</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>552600</xdr:colOff>
+      <xdr:colOff>579240</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -997,8 +1000,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1149120" y="1162440"/>
-        <a:ext cx="5290560" cy="3262320"/>
+        <a:off x="1176120" y="1153440"/>
+        <a:ext cx="5290200" cy="3261960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1960,7 +1963,7 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2202,7 +2205,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2221,7 +2228,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -2477,7 +2484,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,7 +2495,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2506,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,7 +2517,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,7 +2528,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,7 +2539,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,7 +2550,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,7 +2561,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2572,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,7 +2583,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,7 +2594,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,7 +2605,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,7 +2616,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,7 +2627,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,7 +2638,7 @@
         <v>56</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2642,7 +2649,7 @@
         <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,7 +2660,7 @@
         <v>60</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,7 +2671,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,7 +2682,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2686,7 +2693,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,7 +2704,7 @@
         <v>68</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,7 +2715,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,7 +2726,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,7 +2737,7 @@
         <v>74</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2741,205 +2748,205 @@
         <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated team1report to update Sprint 3 progress
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="785" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,11 +18,16 @@
     <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="176">
   <si>
     <t>Initials</t>
   </si>
@@ -310,6 +315,9 @@
   </si>
   <si>
     <t>Unnecessary features</t>
+  </si>
+  <si>
+    <t>Needs acceptance tests</t>
   </si>
   <si>
     <t>Story Description</t>
@@ -560,7 +568,7 @@
     <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -588,12 +596,6 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -704,7 +706,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -783,29 +785,9 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1" sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Burndown Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
-      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
@@ -823,14 +805,57 @@
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="square"/>
             <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4a7ebb"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586">
+                  <a:alpha val="-17698000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln w="6407280">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="6022292400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="6035662080">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -867,13 +892,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
         </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="45722570"/>
-        <c:axId val="72546527"/>
+        <c:axId val="35011038"/>
+        <c:axId val="94529910"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45722570"/>
+        <c:axId val="35011038"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,10 +919,28 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="1" sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Date</a:t>
@@ -897,8 +948,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="MM/DD/YY" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -910,14 +962,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72546527"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="94529910"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72546527"/>
+        <c:axId val="94529910"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,14 +996,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="1" sz="900">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Remaining Stories</a:t>
@@ -941,8 +1029,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -954,8 +1043,27 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45722570"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35011038"/>
         <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -967,6 +1075,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -984,15 +1093,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>410400</xdr:colOff>
+      <xdr:colOff>437400</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>579240</xdr:colOff>
+      <xdr:colOff>605880</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1000,8 +1109,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1176120" y="1153440"/>
-        <a:ext cx="5290200" cy="3261960"/>
+        <a:off x="1189800" y="1144440"/>
+        <a:ext cx="5216760" cy="3261600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1027,10 +1136,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.49553571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.62053571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.875"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.43303571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.44196428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.6607142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,12 +1242,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.25446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.625"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.26785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.15625"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.13392857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.61607142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2767857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9375"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,13 +1663,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.49553571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4955357142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.25446428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3794642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7723214285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3482142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.14285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.90625"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.2232142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,16 +1787,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="22.4955357142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.125"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.1294642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61607142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="22.2053571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.78571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7633928571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.7098214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,17 +2072,17 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.37946428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.37946428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3794642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5848214285714"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.21428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.2276785714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2228,17 +2337,17 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.37946428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1294642857143"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.37946428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8035714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="9.21428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.8660714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,6 +2478,15 @@
       <c r="F6" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2388,6 +2506,15 @@
       </c>
       <c r="F7" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2414,7 +2541,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2470,10 +2597,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.37946428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="137.254464285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.37946428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5848214285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="135.71875"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21428571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2611,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2622,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,7 +2633,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2517,7 +2644,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,7 +2655,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,7 +2666,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2677,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,7 +2688,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2699,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2710,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2721,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2732,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2743,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,7 +2754,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2765,7 @@
         <v>56</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2649,7 +2776,7 @@
         <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2660,7 +2787,7 @@
         <v>60</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2798,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2682,7 +2809,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2693,7 +2820,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2704,7 +2831,7 @@
         <v>68</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,7 +2842,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2726,7 +2853,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2737,7 +2864,7 @@
         <v>74</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2748,205 +2875,205 @@
         <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Team1Report for sprint4 (ahead of schedule)
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="176">
   <si>
     <t>Initials</t>
   </si>
@@ -784,7 +784,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -929,11 +929,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="59770619"/>
-        <c:axId val="82825129"/>
+        <c:axId val="2362824"/>
+        <c:axId val="39372241"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59770619"/>
+        <c:axId val="2362824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,7 +993,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1007,14 +1007,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82825129"/>
+        <c:crossAx val="39372241"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82825129"/>
+        <c:axId val="39372241"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1074,7 @@
           <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1088,9 +1088,8 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59770619"/>
+        <c:crossAx val="2362824"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1120,15 +1119,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>464400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:colOff>491400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>632520</xdr:colOff>
+      <xdr:colOff>659160</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1136,8 +1135,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1207080" y="1135440"/>
-        <a:ext cx="5149800" cy="3261240"/>
+        <a:off x="1224720" y="1126440"/>
+        <a:ext cx="5034960" cy="3260880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1164,8 +1163,9 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,11 +1268,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.01785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9241071428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.89732142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5669642857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.85267857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7008928571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,12 +1689,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2276785714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.02232142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.78571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1026785714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.09375"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2991071428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9910714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.90625"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.66964285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,15 +1813,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="21.96875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.66964285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5267857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.44196428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.91517857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.44196428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.91517857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="21.7321428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2901785714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.32142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.32142857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,8 +2104,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2321428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9910714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.875"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.7589285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2357,14 +2363,17 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4508928571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2142857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6294642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2559,13 +2568,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2991071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50446428571429"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2594,6 +2608,102 @@
       </c>
       <c r="I1" s="8" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2614,14 +2724,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2321428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="134.299107142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.875"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="132.763392857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
implementation and test for US16 -- male surnames in family
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="176">
   <si>
     <t>Initials</t>
   </si>
@@ -929,11 +929,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="2362824"/>
-        <c:axId val="39372241"/>
+        <c:axId val="20406615"/>
+        <c:axId val="75154952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2362824"/>
+        <c:axId val="20406615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,14 +1007,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39372241"/>
+        <c:crossAx val="75154952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39372241"/>
+        <c:axId val="75154952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1088,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2362824"/>
+        <c:crossAx val="20406615"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1119,15 +1119,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>491400</xdr:colOff>
+      <xdr:colOff>518400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>659160</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1135,8 +1135,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1224720" y="1126440"/>
-        <a:ext cx="5034960" cy="3260880"/>
+        <a:off x="1242000" y="1117440"/>
+        <a:ext cx="4958640" cy="3260520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1163,9 +1163,9 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="18.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.8348214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,12 +1268,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.89732142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.37946428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5669642857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7008928571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78125"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.25892857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3303571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5848214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,13 +1689,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.09375"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9910714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.90625"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.66964285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9866071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.7589285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.78571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8660714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,16 +1813,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.37946428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="21.7321428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.55357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2901785714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.67857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.67857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.25892857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="21.4955357142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.43303571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0580357142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.44196428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.44196428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.6473214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,11 +2104,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.875"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.7589285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5223214285714"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5223214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,17 +2363,17 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6294642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9776785714286"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,6 +2492,15 @@
       </c>
       <c r="F5" s="0" t="n">
         <v>45</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,9 +2585,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2991071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9241071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,16 +2733,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="132.763392857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5223214285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="131.227678571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Committing user stories 13 and 14
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr date1904="1" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\SSW-Agile-GEDCOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Backlog" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Burndown" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sprint1" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sprint2" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Sprint3" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Sprint4" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Team" sheetId="1" r:id="rId1"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
+    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
+    <sheet name="Stories" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="176">
   <si>
     <t>Initials</t>
   </si>
@@ -560,15 +564,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="M/D"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -576,39 +578,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -626,7 +600,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -634,93 +608,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -779,29 +701,47 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4a7ebb"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
+                <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -811,16 +751,14 @@
             <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4a7ebb"/>
+                <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
               </a:ln>
@@ -828,10 +766,8 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -839,67 +775,52 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Burndown!$A$2:$A$4</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>mm/dd/yy</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>02/15/16</c:v>
+                  <c:v>40953</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>02/28/16</c:v>
+                  <c:v>40966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>03/13/16</c:v>
+                  <c:v>40980</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -921,6 +842,14 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -929,11 +858,12 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="20406615"/>
-        <c:axId val="75154952"/>
+        <c:smooth val="0"/>
+        <c:axId val="811128880"/>
+        <c:axId val="811129968"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="20406615"/>
+      <c:dateAx>
+        <c:axId val="811128880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,26 +876,26 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
@@ -977,44 +907,46 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="MM/DD/YY" sourceLinked="1"/>
+        <c:numFmt formatCode="mm/dd/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="6480">
             <a:solidFill>
-              <a:srgbClr val="8b8b8b"/>
+              <a:srgbClr val="8B8B8B"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75154952"/>
+        <c:crossAx val="811129968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="75154952"/>
+        <c:axId val="811129968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,26 +959,26 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
@@ -1065,35 +997,38 @@
         <c:spPr>
           <a:ln w="6480">
             <a:solidFill>
-              <a:srgbClr val="8b8b8b"/>
+              <a:srgbClr val="8B8B8B"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20406615"/>
+        <c:crossAx val="811128880"/>
         <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1102,20 +1037,26 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1129,14 +1070,14 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1242000" y="1117440"/>
-        <a:ext cx="4958640" cy="3260520"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1149,26 +1090,284 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.8348214285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.38839285714286"/>
+    <col min="1" max="2" width="5.375"/>
+    <col min="3" max="3" width="7.125"/>
+    <col min="4" max="5" width="17.875"/>
+    <col min="6" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1185,98 +1384,90 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.78125"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.25892857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3303571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5848214285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.38839285714286"/>
+    <col min="1" max="1" width="3.75"/>
+    <col min="2" max="2" width="6.25"/>
+    <col min="3" max="3" width="24.375"/>
+    <col min="4" max="4" width="6.75"/>
+    <col min="5" max="5" width="13.625"/>
+    <col min="6" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1293,412 +1484,403 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>2</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>3</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>4</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>4</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>4</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>4</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.7589285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.78571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.55357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8660714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.38839285714286"/>
+    <col min="2" max="2" width="16.125"/>
+    <col min="3" max="3" width="12.75"/>
+    <col min="4" max="4" width="5.75"/>
+    <col min="5" max="5" width="5.5"/>
+    <col min="6" max="6" width="10.875"/>
+    <col min="7" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -1718,114 +1900,106 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>40953</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>42</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>40966</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">B2-6</f>
+      <c r="B3">
+        <f>B2-6</f>
         <v>36</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <f aca="false">B2-B3</f>
+      <c r="C3">
+        <f>B2-B3</f>
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">SUM(Sprint1!G2:G7)</f>
+      <c r="D3">
+        <f>SUM(Sprint1!G2:G7)</f>
         <v>142</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">MIN(Sprint1!G2:G7)</f>
+      <c r="E3">
+        <f>MIN(Sprint1!G2:G7)</f>
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <f aca="false">(D3-D2)/E3*60</f>
+      <c r="F3" s="5">
+        <f>(D3-D2)/E3*60</f>
         <v>710</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>40980</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <f aca="false">B3-6</f>
+      <c r="B4">
+        <f>B3-6</f>
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <f aca="false">B3-B4</f>
+      <c r="C4">
+        <f>B3-B4</f>
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">SUM(Sprint2!G2:G7)</f>
+      <c r="D4">
+        <f>SUM(Sprint2!G2:G7)</f>
         <v>230</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">MIN(Sprint2!G2:G7)</f>
+      <c r="E4">
+        <f>MIN(Sprint2!G2:G7)</f>
         <v>22</v>
       </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">(D4-D3)/E4*60</f>
+      <c r="F4" s="5">
+        <f>(D4-D3)/E4*60</f>
         <v>240</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.25892857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="21.4955357142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.43303571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0580357142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.44196428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.44196428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.6473214285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.38839285714286"/>
+    <col min="1" max="1" width="6.25"/>
+    <col min="2" max="2" width="21.5" style="6"/>
+    <col min="3" max="3" width="5.375"/>
+    <col min="4" max="4" width="14"/>
+    <col min="5" max="5" width="7.25"/>
+    <col min="6" max="6" width="7.5"/>
+    <col min="7" max="7" width="7.25"/>
+    <col min="8" max="8" width="7.5"/>
+    <col min="9" max="9" width="29.625"/>
+    <col min="10" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1854,264 +2028,256 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>15</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>30</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>33</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>30</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>15</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3">
         <v>30</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>30</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>20</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>20</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5">
         <v>13</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>20</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>30</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>26</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>40</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>10</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>20</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>28</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>5</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5223214285714"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5223214285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.38839285714286"/>
+    <col min="1" max="1" width="8.375"/>
+    <col min="2" max="2" width="27.5"/>
+    <col min="3" max="8" width="8.375"/>
+    <col min="9" max="9" width="12.5"/>
+    <col min="10" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2140,243 +2306,234 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>25</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>22</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>40</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>25</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3">
         <v>33</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>30</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>30</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>25</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4">
         <v>53</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>35</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>30</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>25</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5">
         <v>36</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>40</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>94</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>35</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>44</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>50</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>25</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>42</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>30</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9776785714286"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.38839285714286"/>
+    <col min="1" max="1" width="8.375"/>
+    <col min="2" max="2" width="24"/>
+    <col min="3" max="8" width="8.375"/>
+    <col min="9" max="9" width="10.375"/>
+    <col min="10" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2405,192 +2562,202 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>15</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>35</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>45</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>45</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5">
         <v>19</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>35</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>94</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>45</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>39</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>30</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>20</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>20</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>15</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9241071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.38839285714286"/>
+    <col min="1" max="1" width="8.375"/>
+    <col min="2" max="2" width="24.875"/>
+    <col min="3" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2619,133 +2786,125 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>94</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>30</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5223214285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="131.227678571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.38839285714286"/>
+    <col min="1" max="1" width="8.375"/>
+    <col min="2" max="2" width="27.5"/>
+    <col min="3" max="3" width="131.25" style="6"/>
+    <col min="4" max="1025" width="8.375"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2756,462 +2915,462 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>45</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>72</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>74</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>123</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>125</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>126</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>129</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>131</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>132</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>134</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>135</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>138</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>141</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>144</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>147</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>150</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>153</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>155</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>156</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>158</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>159</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>161</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>162</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>164</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>165</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>167</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>168</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>171</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>174</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -3219,12 +3378,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update team report for sprint 4
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -1,27 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr date1904="1" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\SSW-Agile-GEDCOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Team" sheetId="1" r:id="rId1"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndown" sheetId="3" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
-    <sheet name="Sprint3" sheetId="6" r:id="rId6"/>
-    <sheet name="Sprint4" sheetId="7" r:id="rId7"/>
-    <sheet name="Stories" sheetId="8" r:id="rId8"/>
+    <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Backlog" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Burndown" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sprint1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sprint2" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sprint3" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sprint4" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Stories" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -564,13 +560,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="M/D"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -578,11 +576,39 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -600,7 +626,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -608,41 +634,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -701,47 +779,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4a7ebb"/>
+            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
+                <a:srgbClr val="4a7ebb"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -751,14 +811,16 @@
             <c:size val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4A7EBB"/>
+                <a:srgbClr val="4a7ebb"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
               </a:ln>
@@ -766,61 +828,78 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
-              <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="19080">
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
-              <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="19080">
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Burndown!$A$2:$A$4</c:f>
-              <c:numCache>
-                <c:formatCode>mm/dd/yy</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>40953</c:v>
+                  <c:v>02/15/16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40966</c:v>
+                  <c:v>02/28/16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40980</c:v>
+                  <c:v>03/13/16</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -842,14 +921,6 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -858,12 +929,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="811128880"/>
-        <c:axId val="811129968"/>
+        <c:axId val="27536965"/>
+        <c:axId val="49212139"/>
       </c:lineChart>
-      <c:dateAx>
-        <c:axId val="811128880"/>
+      <c:catAx>
+        <c:axId val="27536965"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,26 +946,26 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
+                        <a:srgbClr val="ffffff"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
+                        <a:srgbClr val="ffffff"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
@@ -907,46 +977,44 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="mm/dd/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="MM/DD/YY" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="6480">
             <a:solidFill>
-              <a:srgbClr val="8B8B8B"/>
+              <a:srgbClr val="8b8b8b"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" strike="noStrike" spc="-1">
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
+                    <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="811129968"/>
+        <c:crossAx val="49212139"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="811129968"/>
+        <c:axId val="49212139"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,26 +1027,26 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:defRPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
+                        <a:srgbClr val="ffffff"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr b="1" sz="900" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
+                        <a:srgbClr val="ffffff"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
@@ -997,38 +1065,35 @@
         <c:spPr>
           <a:ln w="6480">
             <a:solidFill>
-              <a:srgbClr val="8B8B8B"/>
+              <a:srgbClr val="8b8b8b"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" strike="noStrike" spc="-1">
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
+                    <a:srgbClr val="ffffff"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="811128880"/>
+        <c:crossAx val="27536965"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1037,47 +1102,41 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>545400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>145440</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>9720</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="0" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="1231200" y="1107720"/>
+        <a:ext cx="4881960" cy="3260160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1090,284 +1149,26 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="5.375"/>
-    <col min="3" max="3" width="7.125"/>
-    <col min="4" max="5" width="17.875"/>
-    <col min="6" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.5982142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,90 +1185,98 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.75"/>
-    <col min="2" max="2" width="6.25"/>
-    <col min="3" max="3" width="24.375"/>
-    <col min="4" max="4" width="6.75"/>
-    <col min="5" max="5" width="13.625"/>
-    <col min="6" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.66071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.14285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0982142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.61607142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1484,403 +1293,412 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="16.125"/>
-    <col min="3" max="3" width="12.75"/>
-    <col min="4" max="4" width="5.75"/>
-    <col min="5" max="5" width="5.5"/>
-    <col min="6" max="6" width="10.875"/>
-    <col min="7" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5223214285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.66964285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.43303571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -1900,106 +1718,114 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
         <v>40953</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <v>40966</v>
       </c>
-      <c r="B3">
-        <f>B2-6</f>
+      <c r="B3" s="0" t="n">
+        <f aca="false">B2-6</f>
         <v>36</v>
       </c>
-      <c r="C3">
-        <f>B2-B3</f>
+      <c r="C3" s="0" t="n">
+        <f aca="false">B2-B3</f>
         <v>6</v>
       </c>
-      <c r="D3">
-        <f>SUM(Sprint1!G2:G7)</f>
+      <c r="D3" s="0" t="n">
+        <f aca="false">SUM(Sprint1!G2:G7)</f>
         <v>142</v>
       </c>
-      <c r="E3">
-        <f>MIN(Sprint1!G2:G7)</f>
+      <c r="E3" s="0" t="n">
+        <f aca="false">MIN(Sprint1!G2:G7)</f>
         <v>12</v>
       </c>
-      <c r="F3" s="5">
-        <f>(D3-D2)/E3*60</f>
+      <c r="F3" s="5" t="n">
+        <f aca="false">(D3-D2)/E3*60</f>
         <v>710</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>40980</v>
       </c>
-      <c r="B4">
-        <f>B3-6</f>
+      <c r="B4" s="0" t="n">
+        <f aca="false">B3-6</f>
         <v>30</v>
       </c>
-      <c r="C4">
-        <f>B3-B4</f>
+      <c r="C4" s="0" t="n">
+        <f aca="false">B3-B4</f>
         <v>6</v>
       </c>
-      <c r="D4">
-        <f>SUM(Sprint2!G2:G7)</f>
+      <c r="D4" s="0" t="n">
+        <f aca="false">SUM(Sprint2!G2:G7)</f>
         <v>230</v>
       </c>
-      <c r="E4">
-        <f>MIN(Sprint2!G2:G7)</f>
+      <c r="E4" s="0" t="n">
+        <f aca="false">MIN(Sprint2!G2:G7)</f>
         <v>22</v>
       </c>
-      <c r="F4" s="5">
-        <f>(D4-D3)/E4*60</f>
+      <c r="F4" s="5" t="n">
+        <f aca="false">(D4-D3)/E4*60</f>
         <v>240</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.25"/>
-    <col min="2" max="2" width="21.5" style="6"/>
-    <col min="3" max="3" width="5.375"/>
-    <col min="4" max="4" width="14"/>
-    <col min="5" max="5" width="7.25"/>
-    <col min="6" max="6" width="7.5"/>
-    <col min="7" max="7" width="7.25"/>
-    <col min="8" max="8" width="7.5"/>
-    <col min="9" max="9" width="29.625"/>
-    <col min="10" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.14285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="21.2633928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.31696428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.32142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.32142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.2946428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2028,256 +1854,243 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.375"/>
-    <col min="2" max="2" width="27.5"/>
-    <col min="3" max="8" width="8.375"/>
-    <col min="9" max="9" width="12.5"/>
-    <col min="10" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1651785714286"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2306,234 +2119,242 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.375"/>
-    <col min="2" max="2" width="24"/>
-    <col min="3" max="8" width="8.375"/>
-    <col min="9" max="9" width="10.375"/>
-    <col min="10" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7410714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2562,202 +2383,210 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="0" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="0" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.375"/>
-    <col min="2" max="2" width="24.875"/>
-    <col min="3" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5669642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2786,125 +2615,145 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0" t="n">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.375"/>
-    <col min="2" max="2" width="27.5"/>
-    <col min="3" max="3" width="131.25" style="6"/>
-    <col min="4" max="1025" width="8.375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1651785714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="129.8125"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2915,462 +2764,462 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>72</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>123</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>126</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="0" t="s">
         <v>129</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="0" t="s">
         <v>132</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>135</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="0" t="s">
         <v>138</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="0" t="s">
         <v>141</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="0" t="s">
         <v>144</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="0" t="s">
         <v>147</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="0" t="s">
         <v>150</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="0" t="s">
         <v>153</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="0" t="s">
         <v>156</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="0" t="s">
         <v>159</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="0" t="s">
         <v>162</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="0" t="s">
         <v>165</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="0" t="s">
         <v>168</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="0" t="s">
         <v>171</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="0" t="s">
         <v>174</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -3378,7 +3227,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Team1Report for sprint4 progress
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="177">
   <si>
     <t>Initials</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Needs acceptance tests</t>
+  </si>
+  <si>
+    <t>needs acceptance tests</t>
   </si>
   <si>
     <t>Story Description</t>
@@ -929,11 +932,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="27536965"/>
-        <c:axId val="49212139"/>
+        <c:axId val="86196922"/>
+        <c:axId val="23767956"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27536965"/>
+        <c:axId val="86196922"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1007,14 +1010,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49212139"/>
+        <c:crossAx val="23767956"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49212139"/>
+        <c:axId val="23767956"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1091,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27536965"/>
+        <c:crossAx val="86196922"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1119,15 +1122,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>545400</xdr:colOff>
+      <xdr:colOff>572400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>127440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
+      <xdr:colOff>63000</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1135,8 +1138,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1231200" y="1107720"/>
-        <a:ext cx="4881960" cy="3260160"/>
+        <a:off x="1248480" y="1098720"/>
+        <a:ext cx="4805640" cy="3259800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1163,9 +1166,9 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.5982142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85267857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.3616071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,12 +1271,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.66071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.14285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.61607142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.54464285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.02232142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.49553571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3482142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,13 +1692,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5223214285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.66964285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.43303571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8258928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.31696428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6294642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,16 +1816,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.14285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="21.2633928571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.02232142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="20.90625"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.2946428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7008928571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,6 +2031,24 @@
         <v>88</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+    </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7"/>
     </row>
@@ -2048,6 +2069,9 @@
       <c r="B18" s="10" t="s">
         <v>91</v>
       </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
@@ -2083,11 +2107,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.0491071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,11 +2371,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7410714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.15625"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3883928571429"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.92410714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,14 +2600,14 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5669642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3303571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,8 +2726,17 @@
       <c r="F6" s="0" t="n">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>75</v>
       </c>
@@ -2721,6 +2754,15 @@
       </c>
       <c r="F7" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2741,16 +2783,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="129.8125"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="128.392857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,7 +2803,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,7 +2814,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2783,7 +2825,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,7 +2836,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2805,7 +2847,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,7 +2858,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2827,7 +2869,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2838,7 +2880,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,7 +2891,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2860,7 +2902,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2871,7 +2913,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2882,7 +2924,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,7 +2935,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2904,7 +2946,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,7 +2957,7 @@
         <v>56</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,7 +2968,7 @@
         <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2937,7 +2979,7 @@
         <v>60</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,7 +2990,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,7 +3001,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2970,7 +3012,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2981,7 +3023,7 @@
         <v>68</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2992,7 +3034,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3003,7 +3045,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3014,7 +3056,7 @@
         <v>74</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3025,205 +3067,205 @@
         <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement and test US21 -- correct gender for role
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="177">
   <si>
     <t>Initials</t>
   </si>
@@ -932,11 +932,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="86196922"/>
-        <c:axId val="23767956"/>
+        <c:axId val="29589093"/>
+        <c:axId val="10398198"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86196922"/>
+        <c:axId val="29589093"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,14 +1010,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23767956"/>
+        <c:crossAx val="10398198"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23767956"/>
+        <c:axId val="10398198"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1091,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86196922"/>
+        <c:crossAx val="29589093"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1122,15 +1122,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>572400</xdr:colOff>
+      <xdr:colOff>599400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>118440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>63000</xdr:colOff>
+      <xdr:colOff>89640</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>139320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1138,8 +1138,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1248480" y="1098720"/>
-        <a:ext cx="4805640" cy="3259800"/>
+        <a:off x="1266120" y="1089720"/>
+        <a:ext cx="4719240" cy="3259440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1166,9 +1166,8 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.3616071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.125"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,12 +1270,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.54464285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.02232142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8616071428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.49553571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3482142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.42410714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.90625"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5044642857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2276785714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,13 +1690,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8258928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.59375"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.0491071428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.43303571428571"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6294642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,16 +1813,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.02232142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="20.90625"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.90625"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="20.5535714285714"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7008928571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5848214285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85267857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.85267857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.4642857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,11 +2103,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.0491071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8125"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,17 +2358,14 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3883928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.92410714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.03125"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6875"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,15 +2589,13 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3303571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0982142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,6 +2673,15 @@
       </c>
       <c r="F4" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,15 +2781,13 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="128.392857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="126.977678571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
implement and test US22 -- unique IDs
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="177">
   <si>
     <t>Initials</t>
   </si>
@@ -932,11 +932,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="29589093"/>
-        <c:axId val="10398198"/>
+        <c:axId val="70230769"/>
+        <c:axId val="84467689"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29589093"/>
+        <c:axId val="70230769"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,14 +1010,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10398198"/>
+        <c:crossAx val="84467689"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10398198"/>
+        <c:axId val="84467689"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1091,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29589093"/>
+        <c:crossAx val="70230769"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1122,15 +1122,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>599400</xdr:colOff>
+      <xdr:colOff>626400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>89640</xdr:colOff>
+      <xdr:colOff>116280</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1138,8 +1138,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1266120" y="1089720"/>
-        <a:ext cx="4719240" cy="3259440"/>
+        <a:off x="1283400" y="1080720"/>
+        <a:ext cx="4728600" cy="3259080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1166,8 +1166,9 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.125"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.61607142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,11 +1271,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.42410714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.90625"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5044642857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.37946428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2276785714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.30803571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1517857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.25892857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9910714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,12 +1692,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.59375"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.0491071428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.43303571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8125"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="5.31696428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,15 +1815,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.90625"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="20.5535714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.78571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="20.1964285714286"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5848214285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.85267857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.1116071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2103,8 +2106,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5758928571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3392857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6919642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,14 +2364,17 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.03125"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.6875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,13 +2598,15 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0982142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,6 +2713,15 @@
       </c>
       <c r="F5" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2781,13 +2801,15 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5758928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="126.977678571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3392857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="125.558035714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
implement and test US29 and US30
</commit_message>
<xml_diff>
--- a/Team1Report.xlsx
+++ b/Team1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="178">
   <si>
     <t>Initials</t>
   </si>
@@ -320,6 +320,21 @@
     <t>Needs acceptance tests</t>
   </si>
   <si>
+    <t>US29</t>
+  </si>
+  <si>
+    <t>List deceased</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>US30</t>
+  </si>
+  <si>
+    <t>List living married</t>
+  </si>
+  <si>
     <t>needs acceptance tests</t>
   </si>
   <si>
@@ -434,19 +449,7 @@
     <t>List siblings in families by age</t>
   </si>
   <si>
-    <t>US29</t>
-  </si>
-  <si>
-    <t>List deceased</t>
-  </si>
-  <si>
     <t>List all deceased individuals in a GEDCOM file</t>
-  </si>
-  <si>
-    <t>US30</t>
-  </si>
-  <si>
-    <t>List living married</t>
   </si>
   <si>
     <t>List all living married people in a GEDCOM file</t>
@@ -932,11 +935,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="70230769"/>
-        <c:axId val="84467689"/>
+        <c:axId val="38834596"/>
+        <c:axId val="99564268"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70230769"/>
+        <c:axId val="38834596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,14 +1013,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84467689"/>
+        <c:crossAx val="99564268"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84467689"/>
+        <c:axId val="99564268"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1094,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70230769"/>
+        <c:crossAx val="38834596"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1122,15 +1125,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>626400</xdr:colOff>
+      <xdr:colOff>680400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>116280</xdr:colOff>
+      <xdr:colOff>169560</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1138,8 +1141,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1283400" y="1080720"/>
-        <a:ext cx="4728600" cy="3259080"/>
+        <a:off x="1366200" y="1062720"/>
+        <a:ext cx="4594320" cy="3258360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1166,9 +1169,9 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.61607142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.37946428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.4196428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,12 +1274,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.30803571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1517857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.25892857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9910714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.1875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4419642857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.02232142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5223214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,12 +1695,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8839285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5758928571429"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.15625"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.6875"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,16 +1818,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.78571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="20.1964285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.55357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="19.7276785714286"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.31696428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.73214285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.96875"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.1116071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2276785714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.49553571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.49553571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.73214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.4017857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,16 +2104,16 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3392857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6919642857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6294642857143"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,16 +2368,16 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.56696428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0892857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.33035714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,17 +2599,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8616071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1517857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,12 +2641,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>10</v>
@@ -2651,19 +2654,49 @@
       <c r="D2" s="0" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>94</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,7 +2783,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,7 +2812,38 @@
         <v>15</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2800,16 +2864,16 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3392857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="125.558035714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6294642857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="122.723214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2820,7 +2884,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,7 +2895,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2842,7 +2906,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2853,7 +2917,7 @@
         <v>33</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,7 +2928,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,7 +2939,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,7 +2950,7 @@
         <v>39</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2897,7 +2961,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2908,7 +2972,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2919,7 +2983,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2930,7 +2994,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,7 +3005,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2952,7 +3016,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2963,7 +3027,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,7 +3038,7 @@
         <v>56</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2985,7 +3049,7 @@
         <v>58</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2996,7 +3060,7 @@
         <v>60</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3007,7 +3071,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,7 +3082,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3029,7 +3093,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3040,7 +3104,7 @@
         <v>68</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3051,7 +3115,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3062,7 +3126,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3073,7 +3137,7 @@
         <v>74</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3084,205 +3148,205 @@
         <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>